<commit_message>
Evaluation - validate random edges
</commit_message>
<xml_diff>
--- a/figures/robustness_graffs.xlsx
+++ b/figures/robustness_graffs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="23">
   <si>
     <t>DATASET</t>
   </si>
@@ -79,6 +79,9 @@
   <si>
     <t>reproduce</t>
   </si>
+  <si>
+    <t>random-edges</t>
+  </si>
 </sst>
 </file>
 
@@ -3621,6 +3624,720 @@
         <v>21</v>
       </c>
     </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.13445980542754737</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0014184480647895282</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00688916817949076</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002131918260950519</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.016952939533584694</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004879225915811282</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0017129823581436485</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.02304310143346837</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0020423297862322254</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.009752843564973511</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0014184480647895282</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.007121910347716799</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.03985129713306326</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0063271023636877295</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0015714756568415103</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0013097927703334372</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0012847367686077363</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0992089650626236</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004391944531006544</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0012416251168588346</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0026122818635088813</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.4841579347719023</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9814012191322343</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9944865687206641</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.5036312337371162</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9969842790306178</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9969842790306178</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9888328332253828</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9357411374817381</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9291046755137825</v>
+      </c>
+      <c t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Evaluation - unscored networks
</commit_message>
<xml_diff>
--- a/figures/robustness_graffs.xlsx
+++ b/figures/robustness_graffs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="32">
   <si>
     <t>DATASET</t>
   </si>
@@ -82,6 +82,33 @@
   <si>
     <t>random-edges</t>
   </si>
+  <si>
+    <t>random-edges-7</t>
+  </si>
+  <si>
+    <t>airports</t>
+  </si>
+  <si>
+    <t>unscored</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>collab</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>citation</t>
+  </si>
+  <si>
+    <t>random-edges-10</t>
+  </si>
+  <si>
+    <t>unscored-10</t>
+  </si>
 </sst>
 </file>
 
@@ -4338,6 +4365,3814 @@
         <v>22</v>
       </c>
     </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00872317646511195</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00836940836940837</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002690499464693013</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.001573337057208025</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002207128731518975</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00167254206918043</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.001825919289498286</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.14225201321975517</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0017127318956587248</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0022901829353442257</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0020835295225539127</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.006397730483096336</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.05413485509504518</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0033231731068868804</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.007827949901120632</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0841180902156512</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0026720971842923063</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.012338345278903085</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.018563515337708888</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.023717474291056403</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0057845123091305704</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9683158695438046</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.24862164218016602</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.34945840708289694</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.942145170366945</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9867060905870032</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9888328332253828</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9867060905870032</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.8959223656740046</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.889285903706049</v>
+      </c>
+      <c t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0068297331639135955</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002263341804320203</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0042487293519695045</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.011435832274459974</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0013897712833545108</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.3076953621346887</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0010324015247776366</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.6494456860534532</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.059488734835355286</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.008096063382025254</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.8752670144981763</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0062732955712734425</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.5501900331640889</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.011283733597425105</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.005664308983652745</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0029710324337707357</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0068492648137821735</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002166377816291161</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.6256479576680848</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.003697942652540135</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.007353305273582569</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.6959954573118029</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.23141247833622183</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9912863744870954</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004273911895048866</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9279939430824038</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004149179702403662</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9912863744870954</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9994116726386291</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0018001155431434468</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.07632816325261721</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>7.803048162838113E-4</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004921464340950719</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004259811452242599</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>8.145014416986396E-4</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0034424602917593906</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.5981705810238458</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9969509683730763</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9862145733290586</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9877483440496325</v>
+      </c>
+      <c t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0880417073965461</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.008987428194745267</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002059986816084377</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0018153889121631057</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0028487641390867197</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.007127554383651944</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.942145170366945</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.019708606805380998</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.01063166224456547</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9944865687206641</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9683158695438046</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0028953125727319276</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0024072417365100292</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00968207419820323</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9764279021433886</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00320180807985686</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.09555395988322818</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0038149540355250857</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9867060905870032</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0027427253037009135</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.26723289953398005</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0021107626986600187</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9821963712574273</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.014203217513244002</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.05616040822686195</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.025058916329074477</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0021911031473979435</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.007038310221252727</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.1570241950611575</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.8693765178021823</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.8760129797701378</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.3526048284625159</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.003732528589580686</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.006948856416772554</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.010601969504447268</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002104510800508259</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002064803049555273</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.018861181702668362</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9741685290801798</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.005335479078979946</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.5309739383089249</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.011754147066105471</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9912662573834768</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.43876610018281276</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.017058677890566972</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0054441933495729756</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9912662573834768</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.003651894033176529</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.7592677716128758</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.23679747462243128</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00826167346579403</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.006016493998180377</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.19520921020054469</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.006988671382032695</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.009094444281395827</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.16872617146952798</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.014081455805892549</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>26</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.8647216287813309</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9750357781840283</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.010338097613946527</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9669104800324948</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9831610763355619</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>27</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>24</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.3247228430267266</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0012326329069981322</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.004774315225529336</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.08810618052191305</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>12</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.008434779004308257</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.00670357484268257</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.002958914827086836</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.001297010644994987</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="n">
+        <v>0.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.969343095402745</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.42638826031956184</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.966275553961597</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9892821147702064</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>28</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>1.0</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9969509683730763</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>29</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>17</v>
+      </c>
+      <c t="n">
+        <v>0.9984847390936502</v>
+      </c>
+      <c t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>